<commit_message>
completada la parte de bebidas
</commit_message>
<xml_diff>
--- a/Referencias cada 100 de alimento.xlsx
+++ b/Referencias cada 100 de alimento.xlsx
@@ -1,11 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -13,43 +15,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
-    <t>Grupos de alimentos</t>
+    <t xml:space="preserve">Grupos de alimentos</t>
   </si>
   <si>
     <t>Gramos/ml</t>
   </si>
   <si>
-    <t>Kcal totales</t>
-  </si>
-  <si>
-    <t>Carbohidratos (g)</t>
-  </si>
-  <si>
-    <t>Proteínas (g)</t>
-  </si>
-  <si>
-    <t>Grasas totales (g)</t>
-  </si>
-  <si>
-    <t>Alcohol (g)</t>
-  </si>
-  <si>
-    <t>Colesterol (mg)</t>
-  </si>
-  <si>
-    <t>Fibra (g)</t>
+    <t xml:space="preserve">Kcal totales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbohidratos (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteínas (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grasas totales (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcohol (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colesterol (mg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fibra (g)</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>Leche y yogur</t>
+    <t xml:space="preserve">Leche y yogur</t>
   </si>
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>Leche en polvo entera</t>
+    <t xml:space="preserve">Leche en polvo entera</t>
   </si>
   <si>
     <t>A2</t>
@@ -61,25 +63,25 @@
     <t>B</t>
   </si>
   <si>
-    <t>Grasas animales</t>
-  </si>
-  <si>
-    <t>a- Quesos</t>
+    <t xml:space="preserve">Grasas animales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a- Quesos</t>
   </si>
   <si>
     <t>B1</t>
   </si>
   <si>
-    <t>De pasta dura (ej. Sardo, Romano, Provolone, Reggianito, Parmesano)</t>
+    <t xml:space="preserve">De pasta dura (ej. Sardo, Romano, Provolone, Reggianito, Parmesano)</t>
   </si>
   <si>
     <t>B2</t>
   </si>
   <si>
-    <t>De pasta semidura/azul (ej. Holanda, Gouda, Fontina, Pategras, Dambo)</t>
-  </si>
-  <si>
-    <t>b- Cuerpos grasos</t>
+    <t xml:space="preserve">De pasta semidura/azul (ej. Holanda, Gouda, Fontina, Pategras, Dambo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b- Cuerpos grasos</t>
   </si>
   <si>
     <t>B3</t>
@@ -91,37 +93,37 @@
     <t>C</t>
   </si>
   <si>
-    <t>Carnes y huevos</t>
-  </si>
-  <si>
-    <t>a- Huevos</t>
+    <t xml:space="preserve">Carnes y huevos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a- Huevos</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>De gallina entero crudo-hervido- poché</t>
+    <t xml:space="preserve">De gallina entero crudo-hervido- poché</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
-    <t>De gallina entero frito</t>
-  </si>
-  <si>
-    <t>b- Carnes frescas y vísceras</t>
+    <t xml:space="preserve">De gallina entero frito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b- Carnes frescas y vísceras</t>
   </si>
   <si>
     <t>C3</t>
   </si>
   <si>
-    <t>Vacuna magra (ej. bola de lomo, colita de cuadril, cuadril, nalga, tapa de nalga, paleta, cuadrada, peceto, tortuguita y vacío)</t>
+    <t xml:space="preserve">Vacuna magra (ej. bola de lomo, colita de cuadril, cuadril, nalga, tapa de nalga, paleta, cuadrada, peceto, tortuguita y vacío)</t>
   </si>
   <si>
     <t>C4</t>
   </si>
   <si>
-    <t>Vacuna cortes grasos (ej. aguja, bife ancho y angosto, cogote, asado, costillar, entraña, osobuco, matambre, palomita)</t>
+    <t xml:space="preserve">Vacuna cortes grasos (ej. aguja, bife ancho y angosto, cogote, asado, costillar, entraña, osobuco, matambre, palomita)</t>
   </si>
   <si>
     <t>C5</t>
@@ -133,7 +135,7 @@
     <t>D</t>
   </si>
   <si>
-    <t>Carnes procesadas</t>
+    <t xml:space="preserve">Carnes procesadas</t>
   </si>
   <si>
     <t>D1</t>
@@ -145,7 +147,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Salame-salamín-chorizo seco-longaniza</t>
+    <t xml:space="preserve">Salame-salamín-chorizo seco-longaniza</t>
   </si>
   <si>
     <t>D3</t>
@@ -157,13 +159,13 @@
     <t>E</t>
   </si>
   <si>
-    <t>Platos populares</t>
+    <t xml:space="preserve">Platos populares</t>
   </si>
   <si>
     <t>E1</t>
   </si>
   <si>
-    <t>Papas fritas caseras</t>
+    <t xml:space="preserve">Papas fritas caseras</t>
   </si>
   <si>
     <t>E2</t>
@@ -175,7 +177,7 @@
     <t>E3</t>
   </si>
   <si>
-    <t>Empanadas de carne fritas</t>
+    <t xml:space="preserve">Empanadas de carne fritas</t>
   </si>
   <si>
     <t>E4</t>
@@ -187,7 +189,7 @@
     <t>E5</t>
   </si>
   <si>
-    <t>Pastel de papas</t>
+    <t xml:space="preserve">Pastel de papas</t>
   </si>
   <si>
     <t>E6</t>
@@ -223,31 +225,31 @@
     <t>O</t>
   </si>
   <si>
-    <t>Bebidas e infusiones azucaradas</t>
+    <t xml:space="preserve">Bebidas e infusiones azucaradas</t>
   </si>
   <si>
     <t>O1</t>
   </si>
   <si>
-    <t>Aguas saborizadas clásicas</t>
+    <t xml:space="preserve">Aguas saborizadas clásicas</t>
   </si>
   <si>
     <t>O2</t>
   </si>
   <si>
-    <t>Bebidas deportivas y energizantes</t>
+    <t xml:space="preserve">Bebidas deportivas y energizantes</t>
   </si>
   <si>
     <t>O3</t>
   </si>
   <si>
-    <t>Gaseosas clásicas</t>
+    <t xml:space="preserve">Gaseosas clásicas</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>Bebidas alcohólicas</t>
+    <t xml:space="preserve">Bebidas alcohólicas</t>
   </si>
   <si>
     <t>R1</t>
@@ -259,7 +261,7 @@
     <t>R2</t>
   </si>
   <si>
-    <t>Cerveza o aperitivos</t>
+    <t xml:space="preserve">Cerveza o aperitivos</t>
   </si>
   <si>
     <t>R3</t>
@@ -271,46 +273,52 @@
     <t>R4</t>
   </si>
   <si>
-    <t>Bebidas blancas</t>
+    <t xml:space="preserve">Bebidas blancas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B3"/>
         <bgColor rgb="FFC5E0B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
       </patternFill>
     </fill>
     <fill>
@@ -321,112 +329,385 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal style="none"/>
     </border>
     <border>
+      <left style="none"/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf fontId="2" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -483,7 +764,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -509,7 +790,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -561,16 +842,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -586,7 +879,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -616,21 +909,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.38"/>
-    <col customWidth="1" min="2" max="2" width="92.38"/>
+    <col customWidth="1" min="1" max="1" width="4.3799999999999999"/>
+    <col customWidth="1" min="2" max="2" width="92.379999999999995"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -687,69 +984,69 @@
         <v>12</v>
       </c>
       <c r="C3" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D4" si="1">(E3*4)+(F3*4)+(G3*9)+(H3*7)</f>
-        <v>494.04</v>
+        <f t="shared" ref="D3:D8" si="0">(E3*4)+(F3*4)+(G3*9)+(H3*7)</f>
+        <v>494.04000000000002</v>
       </c>
       <c r="E3" s="8">
-        <v>38.05</v>
+        <v>38.049999999999997</v>
       </c>
       <c r="F3" s="8">
-        <v>26.15</v>
+        <v>26.149999999999999</v>
       </c>
       <c r="G3" s="8">
-        <v>26.36</v>
+        <v>26.359999999999999</v>
       </c>
       <c r="H3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>80.48</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>80.480000000000004</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="1"/>
-        <v>57.92</v>
+        <f t="shared" si="0"/>
+        <v>57.920000000000002</v>
       </c>
       <c r="E4" s="8">
-        <v>4.63</v>
+        <v>4.6299999999999999</v>
       </c>
       <c r="F4" s="8">
-        <v>3.1</v>
+        <v>3.1000000000000001</v>
       </c>
       <c r="G4" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>10.11</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>10.109999999999999</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5"/>
@@ -762,130 +1059,130 @@
       <c r="J5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" ref="D7:D8" si="2">(E7*4)+(F7*4)+(G7*9)+(H7*7)</f>
-        <v>373.83</v>
+        <f t="shared" si="0"/>
+        <v>373.82999999999998</v>
       </c>
       <c r="E7" s="8">
-        <v>0.34</v>
+        <v>0.34000000000000002</v>
       </c>
       <c r="F7" s="8">
-        <v>32.39</v>
+        <v>32.390000000000001</v>
       </c>
       <c r="G7" s="8">
-        <v>26.99</v>
+        <v>26.989999999999998</v>
       </c>
       <c r="H7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>82.99</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>82.989999999999995</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="2"/>
-        <v>328.16</v>
+        <f t="shared" si="0"/>
+        <v>328.16000000000003</v>
       </c>
       <c r="E8" s="8">
-        <v>0.1</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="F8" s="8">
-        <v>25.33</v>
+        <v>25.329999999999998</v>
       </c>
       <c r="G8" s="8">
         <v>25.16</v>
       </c>
       <c r="H8" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>72.14</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>72.140000000000001</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D10" s="8">
         <f>(E10*4)+(F10*4)+(G10*9)+(H10*7)</f>
-        <v>745.35</v>
+        <v>745.35000000000002</v>
       </c>
       <c r="E10" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="8">
-        <v>0.33</v>
+        <v>0.33000000000000002</v>
       </c>
       <c r="G10" s="8">
-        <v>82.67</v>
+        <v>82.670000000000002</v>
       </c>
       <c r="H10" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>223.0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>223</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -905,18 +1202,18 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
@@ -926,29 +1223,29 @@
         <v>29</v>
       </c>
       <c r="C13" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13:D14" si="3">(E13*4)+(F13*4)+(G13*9)+(H13*7)</f>
+        <f t="shared" ref="D13:D42" si="1">(E13*4)+(F13*4)+(G13*9)+(H13*7)</f>
         <v>153.75</v>
       </c>
       <c r="E13" s="8">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="F13" s="8">
-        <v>12.7</v>
+        <v>12.699999999999999</v>
       </c>
       <c r="G13" s="8">
         <v>11.35</v>
       </c>
       <c r="H13" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>449.0</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>449</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -959,146 +1256,146 @@
         <v>31</v>
       </c>
       <c r="C14" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="3"/>
-        <v>191.32</v>
+        <f t="shared" si="1"/>
+        <v>191.31999999999999</v>
       </c>
       <c r="E14" s="8">
-        <v>0.83</v>
+        <v>0.82999999999999996</v>
       </c>
       <c r="F14" s="8">
-        <v>13.61</v>
+        <v>13.609999999999999</v>
       </c>
       <c r="G14" s="8">
         <v>14.84</v>
       </c>
       <c r="H14" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I14" s="9">
-        <v>401.0</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>401</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" ref="D16:D18" si="4">(E16*4)+(F16*4)+(G16*9)+(H16*7)</f>
-        <v>130.6</v>
+        <f t="shared" si="1"/>
+        <v>130.59999999999999</v>
       </c>
       <c r="E16" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F16" s="8">
-        <v>21.4</v>
+        <v>21.399999999999999</v>
       </c>
       <c r="G16" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>62.31</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>62.310000000000002</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" si="4"/>
-        <v>199.55</v>
+        <f t="shared" si="1"/>
+        <v>199.55000000000001</v>
       </c>
       <c r="E17" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F17" s="8">
-        <v>18.95</v>
+        <v>18.949999999999999</v>
       </c>
       <c r="G17" s="8">
         <v>13.75</v>
       </c>
       <c r="H17" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>68.34</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>68.340000000000003</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D18" s="8">
-        <f t="shared" si="4"/>
-        <v>165.075</v>
+        <f t="shared" si="1"/>
+        <v>165.07499999999999</v>
       </c>
       <c r="E18" s="8">
-        <f t="shared" ref="E18:G18" si="5">AVERAGE(E16:E17)</f>
+        <f t="shared" ref="E18:G18" si="2">AVERAGE(E16:E17)</f>
         <v>0</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="5"/>
-        <v>20.175</v>
+        <f t="shared" si="2"/>
+        <v>20.175000000000001</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>9.375</v>
       </c>
       <c r="H18" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I18" s="8">
-        <f t="shared" ref="I18:J18" si="6">AVERAGE(I16:I17)</f>
-        <v>65.325</v>
+        <f t="shared" ref="I18:J18" si="3">AVERAGE(I16:I17)</f>
+        <v>65.325000000000003</v>
       </c>
       <c r="J18" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1126,11 +1423,11 @@
         <v>42</v>
       </c>
       <c r="C20" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D20" s="8">
-        <f t="shared" ref="D20:D22" si="7">(E20*4)+(F20*4)+(G20*9)+(H20*7)</f>
-        <v>187.92</v>
+        <f t="shared" si="1"/>
+        <v>187.91999999999999</v>
       </c>
       <c r="E20" s="8">
         <v>5.75</v>
@@ -1139,16 +1436,16 @@
         <v>12.25</v>
       </c>
       <c r="G20" s="8">
-        <v>12.88</v>
+        <v>12.880000000000001</v>
       </c>
       <c r="H20" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I20" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="J20" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>30</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1159,29 +1456,29 @@
         <v>44</v>
       </c>
       <c r="C21" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D21" s="8">
-        <f t="shared" si="7"/>
-        <v>377.45</v>
+        <f t="shared" si="1"/>
+        <v>377.44999999999999</v>
       </c>
       <c r="E21" s="8">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F21" s="8">
-        <v>19.53</v>
+        <v>19.530000000000001</v>
       </c>
       <c r="G21" s="8">
-        <v>33.13</v>
+        <v>33.130000000000003</v>
       </c>
       <c r="H21" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I21" s="9">
-        <v>78.0</v>
-      </c>
-      <c r="J21" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>78</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1192,36 +1489,36 @@
         <v>46</v>
       </c>
       <c r="C22" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D22" s="8">
-        <f t="shared" si="7"/>
-        <v>265.24</v>
+        <f t="shared" si="1"/>
+        <v>265.24000000000001</v>
       </c>
       <c r="E22" s="8">
-        <v>1.56</v>
+        <v>1.5600000000000001</v>
       </c>
       <c r="F22" s="8">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="G22" s="8">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="H22" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I22" s="9">
-        <v>71.0</v>
-      </c>
-      <c r="J22" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>71</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="5"/>
@@ -1234,54 +1531,54 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C24" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D24" s="8">
-        <f t="shared" ref="D24:D29" si="8">(E24*4)+(F24*4)+(G24*9)+(H24*7)</f>
-        <v>162.04</v>
+        <f t="shared" si="1"/>
+        <v>162.03999999999999</v>
       </c>
       <c r="E24" s="8">
-        <v>17.49</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="F24" s="8">
-        <v>2.05</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G24" s="8">
-        <v>9.32</v>
+        <v>9.3200000000000003</v>
       </c>
       <c r="H24" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I24" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J24" s="9">
-        <v>2.4</v>
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8">
+        <v>2.3999999999999999</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D25" s="8">
-        <f t="shared" si="8"/>
-        <v>251.86</v>
+        <f t="shared" si="1"/>
+        <v>251.86000000000001</v>
       </c>
       <c r="E25" s="8">
-        <v>26.49</v>
+        <v>26.489999999999998</v>
       </c>
       <c r="F25" s="8">
         <v>13.57</v>
@@ -1290,145 +1587,145 @@
         <v>10.18</v>
       </c>
       <c r="H25" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I25" s="9">
-        <v>17.0</v>
-      </c>
-      <c r="J25" s="9">
-        <v>2.3</v>
+        <v>0</v>
+      </c>
+      <c r="I25" s="8">
+        <v>17</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C26" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D26" s="8">
-        <f t="shared" si="8"/>
-        <v>297.48</v>
+        <f t="shared" si="1"/>
+        <v>297.48000000000002</v>
       </c>
       <c r="E26" s="8">
         <v>14.82</v>
       </c>
       <c r="F26" s="8">
-        <v>10.14</v>
+        <v>10.140000000000001</v>
       </c>
       <c r="G26" s="8">
-        <v>21.96</v>
+        <v>21.960000000000001</v>
       </c>
       <c r="H26" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I26" s="9">
-        <v>68.94</v>
-      </c>
-      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8">
+        <v>68.939999999999998</v>
+      </c>
+      <c r="J26" s="8">
         <v>0.62</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D27" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>214.41</v>
       </c>
       <c r="E27" s="8">
         <v>14.82</v>
       </c>
       <c r="F27" s="8">
-        <v>10.14</v>
+        <v>10.140000000000001</v>
       </c>
       <c r="G27" s="8">
         <v>12.73</v>
       </c>
       <c r="H27" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I27" s="9">
-        <v>68.94</v>
-      </c>
-      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <v>68.939999999999998</v>
+      </c>
+      <c r="J27" s="8">
         <v>0.62</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C28" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D28" s="8">
-        <f t="shared" si="8"/>
-        <v>143.32</v>
+        <f t="shared" si="1"/>
+        <v>143.31999999999999</v>
       </c>
       <c r="E28" s="8">
-        <v>7.69</v>
+        <v>7.6900000000000004</v>
       </c>
       <c r="F28" s="8">
-        <v>8.34</v>
+        <v>8.3399999999999999</v>
       </c>
       <c r="G28" s="8">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H28" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I28" s="9">
-        <v>68.52</v>
-      </c>
-      <c r="J28" s="9">
-        <v>0.98</v>
+        <v>0</v>
+      </c>
+      <c r="I28" s="8">
+        <v>68.519999999999996</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.97999999999999998</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D29" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>100.08</v>
       </c>
       <c r="E29" s="8">
         <v>12.44</v>
       </c>
       <c r="F29" s="8">
-        <v>5.47</v>
+        <v>5.4699999999999998</v>
       </c>
       <c r="G29" s="8">
-        <v>3.16</v>
+        <v>3.1600000000000001</v>
       </c>
       <c r="H29" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I29" s="9">
-        <v>14.39</v>
-      </c>
-      <c r="J29" s="9">
-        <v>4.02</v>
+        <v>0</v>
+      </c>
+      <c r="I29" s="8">
+        <v>14.390000000000001</v>
+      </c>
+      <c r="J29" s="8">
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="30">
@@ -1455,29 +1752,29 @@
         <v>64</v>
       </c>
       <c r="C31" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D31" s="8">
-        <f t="shared" ref="D31:D33" si="9">(E31*4)+(F31*4)+(G31*9)+(H31*7)</f>
-        <v>98.69</v>
+        <f t="shared" si="1"/>
+        <v>98.689999999999998</v>
       </c>
       <c r="E31" s="8">
         <v>22.84</v>
       </c>
       <c r="F31" s="8">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="G31" s="8">
-        <v>0.33</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="I31" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J31" s="9">
-        <v>2.6</v>
+        <v>0.33000000000000002</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0</v>
+      </c>
+      <c r="J31" s="8">
+        <v>2.6000000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -1488,28 +1785,28 @@
         <v>66</v>
       </c>
       <c r="C32" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D32" s="8">
-        <f t="shared" si="9"/>
-        <v>46.47</v>
+        <f t="shared" si="1"/>
+        <v>46.469999999999999</v>
       </c>
       <c r="E32" s="8">
         <v>10.1</v>
       </c>
       <c r="F32" s="8">
-        <v>0.91</v>
+        <v>0.91000000000000003</v>
       </c>
       <c r="G32" s="8">
-        <v>0.27</v>
-      </c>
-      <c r="H32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="I32" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J32" s="9">
+        <v>0.27000000000000002</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0</v>
+      </c>
+      <c r="J32" s="8">
         <v>1.5</v>
       </c>
     </row>
@@ -1521,29 +1818,29 @@
         <v>68</v>
       </c>
       <c r="C33" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D33" s="8">
-        <f t="shared" si="9"/>
-        <v>58.2</v>
+        <f t="shared" si="1"/>
+        <v>58.200000000000003</v>
       </c>
       <c r="E33" s="8">
-        <v>13.8</v>
+        <v>13.800000000000001</v>
       </c>
       <c r="F33" s="8">
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="G33" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="H33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="I33" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J33" s="9">
-        <v>2.4</v>
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+      <c r="J33" s="8">
+        <v>2.3999999999999999</v>
       </c>
     </row>
     <row r="34">
@@ -1570,29 +1867,29 @@
         <v>72</v>
       </c>
       <c r="C35" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D35" s="8">
-        <f t="shared" ref="D35:D37" si="10">(E35*4)+(F35*4)+(G35*9)+(H35*7)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="E35" s="8">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F35" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G35" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H35" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I35" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J35" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1603,29 +1900,29 @@
         <v>74</v>
       </c>
       <c r="C36" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D36" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="E36" s="8">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F36" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G36" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H36" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I36" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J36" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="J36" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1636,36 +1933,36 @@
         <v>76</v>
       </c>
       <c r="C37" s="8">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D37" s="8">
-        <f t="shared" si="10"/>
-        <v>42.96</v>
+        <f t="shared" si="1"/>
+        <v>42.960000000000001</v>
       </c>
       <c r="E37" s="8">
         <v>10.74</v>
       </c>
       <c r="F37" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G37" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H37" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I37" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J37" s="9">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C38" s="5"/>
@@ -1681,135 +1978,138 @@
       <c r="A39" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="8">
-        <v>100.0</v>
-      </c>
-      <c r="D39" s="9">
-        <f t="shared" ref="D39:D42" si="11">(E39*4)+(F39*4)+(G39*9)+(H39*7)</f>
-        <v>86.59</v>
-      </c>
-      <c r="E39" s="9">
-        <v>3.17</v>
-      </c>
-      <c r="F39" s="9">
+        <v>100</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" si="1"/>
+        <v>86.590000000000003</v>
+      </c>
+      <c r="E39" s="8">
+        <v>3.1699999999999999</v>
+      </c>
+      <c r="F39" s="8">
         <v>0.19</v>
       </c>
-      <c r="G39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="9">
-        <v>10.45</v>
-      </c>
-      <c r="I39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J39" s="9">
-        <v>0.0</v>
+      <c r="G39" s="8">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
+        <v>10.449999999999999</v>
+      </c>
+      <c r="I39" s="8">
+        <v>0</v>
+      </c>
+      <c r="J39" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C40" s="8">
-        <v>100.0</v>
-      </c>
-      <c r="D40" s="9">
-        <f t="shared" si="11"/>
-        <v>35.48</v>
-      </c>
-      <c r="E40" s="9">
-        <v>1.61</v>
-      </c>
-      <c r="F40" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="G40" s="9">
-        <v>0.06</v>
-      </c>
-      <c r="H40" s="9">
-        <v>3.9</v>
-      </c>
-      <c r="I40" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J40" s="9">
-        <v>0.0</v>
+        <v>100</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" si="1"/>
+        <v>35.479999999999997</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1.6100000000000001</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="H40" s="8">
+        <v>3.8999999999999999</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0</v>
+      </c>
+      <c r="J40" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C41" s="8">
-        <v>100.0</v>
-      </c>
-      <c r="D41" s="9">
-        <f t="shared" si="11"/>
-        <v>370.35</v>
-      </c>
-      <c r="E41" s="9">
+        <v>100</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="1"/>
+        <v>370.35000000000002</v>
+      </c>
+      <c r="E41" s="8">
         <v>46.75</v>
       </c>
-      <c r="F41" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="G41" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="H41" s="9">
+      <c r="F41" s="8">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="H41" s="8">
         <v>25.75</v>
       </c>
-      <c r="I41" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J41" s="9">
-        <v>0.0</v>
+      <c r="I41" s="8">
+        <v>0</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C42" s="8">
-        <v>100.0</v>
-      </c>
-      <c r="D42" s="9">
-        <f t="shared" si="11"/>
-        <v>233.8</v>
-      </c>
-      <c r="E42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="F42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="G42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H42" s="9">
-        <v>33.4</v>
-      </c>
-      <c r="I42" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J42" s="9">
-        <v>0.0</v>
+        <v>100</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" si="1"/>
+        <v>233.80000000000001</v>
+      </c>
+      <c r="E42" s="8">
+        <v>0</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8">
+        <v>33.399999999999999</v>
+      </c>
+      <c r="I42" s="8">
+        <v>0</v>
+      </c>
+      <c r="J42" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>